<commit_message>
Modified two files CheckListAudioCataloger.xlsx and Audio_Cataloger_Requirements.pdf
</commit_message>
<xml_diff>
--- a/CheckListAudioCataloger.xlsx
+++ b/CheckListAudioCataloger.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD48004E-9A3E-4BDB-AB7D-C787042D2990}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2991A62E-AC51-4179-9CEE-DEF91056A46B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="602" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="54">
   <si>
     <t>Requirements No.</t>
   </si>
@@ -375,30 +375,228 @@
     <t>directory not available</t>
   </si>
   <si>
-    <t>Start with directory available HTML CSW</t>
-  </si>
-  <si>
-    <t>Start with directory available HTML CSW parameters. Directory conteints files: mp3 flac wav. No nested directory, no broken file.</t>
-  </si>
-  <si>
     <t>Peparation</t>
   </si>
   <si>
+    <t>1. Start program. Parameters: 
+    StartingDirectory (new directory), 
+    HtmlOutputFileName,
+    CsvOutputFileName.
+2. Wait until the program finishes.
+3. Stop application Ctrl+C.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Windows.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Start with directory available 
+HTML CSW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Windows.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Start with directory available 
+HTML CSW. Directory contains broken files.</t>
+    </r>
+  </si>
+  <si>
+    <t>Start with directory available HTML CSW parameters. Directory conteints files: mp3 flac wav. Directory conteints duplicates. No nested directory, no broken file.</t>
+  </si>
+  <si>
+    <t>Start with directory available HTML CSW parameters. Directory conteints files: mp3 flac wav, broken files. Directory conteints duplicates.  No nested directory.</t>
+  </si>
+  <si>
     <t>1. Create new directory.
-2. Add files: mp3, flac, wav.</t>
+2. Add files: mp3, flac, wav.
+3. Add duplicates.</t>
+  </si>
+  <si>
+    <t>1. Create new directory.
+2. Add files: mp3, flac, wav.
+3. Add duplicates.
+4. Add broken files.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Windows.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Start with directory inavailable 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Start with directory inavailable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Start program. Parameters: 
+    Wrong name directory (new directory), 
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Error messag: “The following directory is not found or is inaccessible: {full path}”
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Windows.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Start with directory available 
+HTML CSW. Directory contains nested directory.</t>
+    </r>
+  </si>
+  <si>
+    <t>Start with directory available HTML CSW parameters. Directory conteints files: mp3 flac wav. Directory conteints duplicates, nested directory, no broken file.</t>
+  </si>
+  <si>
+    <t>1. Create new directory.
+2. Add files: mp3, flac, wav.
+3. Add duplicates.
+4. Add nested directory with audio files.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Windows.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Start with directory available 
+HTML CSW. DuplicatesOnly mode.</t>
+    </r>
+  </si>
+  <si>
+    <t>Start with directory available HTML CSW, DuplicatesOnly mode parameters. Directory conteints files: mp3 flac wav. Directory conteints duplicates. No nested directory, no broken file.</t>
   </si>
   <si>
     <t>1. Start program. Parameters: 
-  StartingDirectory (new directory), 
-  HtmlOutputFileName,
-  CsvOutputFileName.</t>
+    StartingDirectory (new directory), 
+    DuplicatesOnly
+    HtmlOutputFileName,
+    CsvOutputFileName.
+2. Wait until the program finishes.
+3. Stop application Ctrl+C.</t>
+  </si>
+  <si>
+    <t>1. The program starts with the specified parameters.
+2. HTML (for browser) and CSV (for spreadsheet editor) output.
+3. The program stops.
+4. Created a list of all audio files in the specified directory.
+5.Background for duplicates should be red.
+6. The application should display its current activity in the console.</t>
+  </si>
+  <si>
+    <t>1. The program starts with the specified parameters.
+2. HTML (for browser) and CSV (for spreadsheet editor) output.
+3. The program stops.
+4. Created a list of all audio files in the specified and nested directory.
+5.Background for duplicates should be red.
+6. The application should display its current activity in the console.</t>
+  </si>
+  <si>
+    <t>1. The program starts with the specified parameters.
+2. HTML (for browser) and CSV (for spreadsheet editor) output.
+3. The program stops.
+4. Created a list of all audio files in the specified directory.
+5. The background color for duplicates should be white in HTML output. 
+6. The application should display its current activity in the console.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The program starts with the specified parameters/
+2. HTML (for browser) and CSV (for spreadsheet editor) output.
+3. The program stops.
+4. Created a list of all audio files in the specified directory.
+5.Background for duplicates should be red.
+6. The application should display its current activity in the console.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>7. No matter how broken an audio file is, the application should either extract necessary data or replace the data with predefined stubs in the output. Error messag “The following file is not writable: {full path}”.
+7. If a broken file or a file with unsupported inner structure detected, the application should display a log message “No audio header or audio tag data in: {full path}”.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -481,6 +679,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -517,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -565,27 +770,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -956,8 +1160,11 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
       <c r="H2" t="s">
         <v>24</v>
       </c>
@@ -966,15 +1173,12 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="24" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="I3" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1065,10 +1269,10 @@
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1159,10 +1363,10 @@
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="24" t="s">
+      <c r="I27" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1253,10 +1457,10 @@
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D39" s="24" t="s">
+      <c r="D39" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="24" t="s">
+      <c r="I39" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1343,19 +1547,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C3B29E-3101-4936-BDD9-1C4E28535B1E}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="19" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="4" width="43.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60.5703125" customWidth="1"/>
-    <col min="6" max="7" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" customWidth="1"/>
+    <col min="6" max="6" width="66.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
@@ -1363,106 +1568,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="F2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="18"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="C4" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" s="24" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="24"/>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
+      <c r="D35" s="20"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>